<commit_message>
Moves pFBA function into transAnalysis, updated data sources
</commit_message>
<xml_diff>
--- a/data/data_sources.xlsx
+++ b/data/data_sources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="18140" windowHeight="17920" tabRatio="500"/>
+    <workbookView xWindow="17840" yWindow="3400" windowWidth="18140" windowHeight="17920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>The HUGE precurser file came from a cuff diff including bop27 data, which was identical to the second anaerobe2 fpkm file, so I assumed the HUGE data was under similar conditions. Also it's minspan fpkm averages line up well with the anerobic data.</t>
   </si>
@@ -161,6 +161,46 @@
   </si>
   <si>
     <t>Aerobic/Anaerobic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>an_isoforms.fpkm_tracking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RNAseq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anaerobic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glucose?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M9?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WT?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bop27?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arvsan_isoforms.fpkm_tracking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RNAseq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aerobic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -168,12 +208,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -574,7 +608,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:I15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -771,6 +805,52 @@
         <v>34</v>
       </c>
     </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>1</v>
@@ -845,7 +925,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>